<commit_message>
updated a spelling mistake
</commit_message>
<xml_diff>
--- a/data/demoqa/demoqa_submit_form_data.xlsx
+++ b/data/demoqa/demoqa_submit_form_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\UI_Automation_RobotFramework\robot-framework-ui-test-repo\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\UI_Automation_RobotFramework\robot-framework-ui-test-repo\data\demoqa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DA606B-50C5-4698-B235-284C991DD666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FE8C5A-36E2-4879-A397-08B5C2EE5C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E197D71B-7F08-47D8-A720-D734CE53A151}"/>
   </bookViews>
@@ -60,7 +60,7 @@
     <t>textbox</t>
   </si>
   <si>
-    <t>Test Box Interactions</t>
+    <t>Text Box Interactions</t>
   </si>
 </sst>
 </file>
@@ -109,11 +109,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,7 +430,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,7 +470,7 @@
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">

</xml_diff>